<commit_message>
Resolve PA-27 issues - refactor method namings, change stream forech to fori loop
</commit_message>
<xml_diff>
--- a/List_of_Reports.xlsx
+++ b/List_of_Reports.xlsx
@@ -98,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false" zoomScale="130">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -120,24 +120,145 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n" s="3">
-        <v>44860.0</v>
+        <v>44562.0</v>
       </c>
       <c r="C2" t="n" s="3">
-        <v>44860.0</v>
+        <v>44926.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="2">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="n" s="3">
-        <v>44860.0</v>
+        <v>44562.0</v>
       </c>
       <c r="C3" t="n" s="3">
-        <v>44860.0</v>
+        <v>44926.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n" s="3">
+        <v>44562.0</v>
+      </c>
+      <c r="C4" t="n" s="3">
+        <v>44926.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n" s="3">
+        <v>44562.0</v>
+      </c>
+      <c r="C5" t="n" s="3">
+        <v>44926.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n" s="3">
+        <v>44562.0</v>
+      </c>
+      <c r="C6" t="n" s="3">
+        <v>47848.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n" s="3">
+        <v>44562.0</v>
+      </c>
+      <c r="C7" t="n" s="3">
+        <v>47848.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n" s="3">
+        <v>44563.0</v>
+      </c>
+      <c r="C8" t="n" s="3">
+        <v>47847.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n" s="3">
+        <v>44574.0</v>
+      </c>
+      <c r="C9" t="n" s="3">
+        <v>47847.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n" s="3">
+        <v>44574.0</v>
+      </c>
+      <c r="C10" t="n" s="3">
+        <v>46021.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n" s="3">
+        <v>44755.0</v>
+      </c>
+      <c r="C11" t="n" s="3">
+        <v>46021.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n" s="3">
+        <v>44755.0</v>
+      </c>
+      <c r="C12" t="n" s="3">
+        <v>46015.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n" s="3">
+        <v>44754.0</v>
+      </c>
+      <c r="C13" t="n" s="3">
+        <v>46015.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="n" s="3">
+        <v>44024.0</v>
+      </c>
+      <c r="C14" t="n" s="3">
+        <v>46015.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>